<commit_message>
fix: FINAL - restore clean two-dataset baseline in data/processed/ - Successfully recover R&D.xlsx (1.3MB) from Git history using raw object syntax - Confirm corrected revenue&profit rate.xlsx (10KB) is in place - Remove residual empty file - Enforce strict .gitignore to prevent future clutter
</commit_message>
<xml_diff>
--- a/data/processed/revenue&profit rate.xlsx
+++ b/data/processed/revenue&profit rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tesla-optimus-business-analysis\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A2CE1C-AD5C-4265-8E78-08C58677C3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56782692-0EAF-4CB1-971A-6E74CD34743C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="13612" windowHeight="10522" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Revenues</t>
   </si>
@@ -731,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:W1048576"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -836,9 +836,7 @@
       <c r="J4" s="52"/>
       <c r="K4" s="26"/>
       <c r="L4" s="34"/>
-      <c r="M4" s="35">
-        <v>1052</v>
-      </c>
+      <c r="M4" s="35"/>
       <c r="N4" s="31"/>
     </row>
     <row r="5" spans="1:14" ht="19.149999999999999">
@@ -865,7 +863,7 @@
       <c r="K5" s="25"/>
       <c r="L5" s="36"/>
       <c r="M5" s="37">
-        <v>27236</v>
+        <v>1052</v>
       </c>
       <c r="N5" s="32"/>
     </row>
@@ -893,7 +891,7 @@
       <c r="K6" s="27"/>
       <c r="L6" s="31"/>
       <c r="M6" s="38">
-        <v>1994</v>
+        <v>27236</v>
       </c>
       <c r="N6" s="31"/>
     </row>
@@ -921,7 +919,7 @@
       <c r="K7" s="25"/>
       <c r="L7" s="39"/>
       <c r="M7" s="40">
-        <v>2306</v>
+        <v>1994</v>
       </c>
       <c r="N7" s="32"/>
     </row>
@@ -949,7 +947,7 @@
       <c r="K8" s="27"/>
       <c r="L8" s="29"/>
       <c r="M8" s="41">
-        <v>31536</v>
+        <v>2306</v>
       </c>
       <c r="N8" s="31"/>
     </row>
@@ -1079,26 +1077,15 @@
         <v>721</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="2:13">
       <c r="B17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
+      <c r="L17" s="39"/>
+      <c r="M17" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="F2:H2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="D11:E11"/>
@@ -1120,6 +1107,7 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="L12:M12"/>

</xml_diff>